<commit_message>
Update literature review excel
</commit_message>
<xml_diff>
--- a/Literature/Literature Review Overview.xlsx
+++ b/Literature/Literature Review Overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/nik_verweel_wur_nl/Documents/MSc/Year 2/Thesis/Thesis Submission Folder/Literature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nik Verweel\Documents\Git Repos\msc-thesis-digital-appendix\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{AF52B1AB-7F27-4E92-B698-A04AFEB486E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CF2BFBF-2EB1-4CBB-BC9C-37BEB8F9ECAD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFC78A2-F701-4770-865F-4DE48E0E5005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2639,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W88" sqref="W88"/>
+    <sheetView tabSelected="1" topLeftCell="P6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4102,11 +4102,11 @@
         <v>8</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="T27" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="U27" s="6" t="s">
         <v>529</v>

</xml_diff>